<commit_message>
Ready for production (just for now)
</commit_message>
<xml_diff>
--- a/lib/files/courses.xlsx
+++ b/lib/files/courses.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t xml:space="preserve">Arquitetura e Urbanismo</t>
   </si>
@@ -181,6 +181,21 @@
   </si>
   <si>
     <t xml:space="preserve">Engenharia Industrial Madeireira Noturno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engenharia Civil, Ciência da Computação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciatura em Química Noturno, Matemática Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Física Noturno, Matemática Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matemática Diurno, Matemática Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matemática Industrial, Engenharia Industrial Madeireira Diurno</t>
   </si>
   <si>
     <t xml:space="preserve">PGMAT</t>
@@ -569,10 +584,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1032,7 +1047,7 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>53</v>
@@ -1040,7 +1055,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>54</v>
@@ -1048,7 +1063,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>55</v>
@@ -1056,12 +1071,71 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.236111111111111" right="0.236111111111111" top="0.236111111111111" bottom="0.236111111111111" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>